<commit_message>
Version 1.4.2 minor fix
</commit_message>
<xml_diff>
--- a/input_second.xlsx
+++ b/input_second.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new\printing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BB0C3F-B512-4FF3-BFD4-9800E8656DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE4C08D-5B18-4525-8C3D-611EEA1F9DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -105,9 +114,6 @@
     <t>периодическая</t>
   </si>
   <si>
-    <t>Установка для поверки каналов измерения давления и частоты пульса УПКД-3</t>
-  </si>
-  <si>
     <t>66733.17.3P.00551601</t>
   </si>
   <si>
@@ -151,6 +157,9 @@
   </si>
   <si>
     <t>Все атрибуты должны идти друг под другом БЕЗ пустых ячеек, поскольку при встрече пустой ячейки, все остальные ИГНОРИРУЮТСЯ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -485,7 +494,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +544,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -558,16 +567,16 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
         <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
       </c>
       <c r="K2">
         <v>3</v>
@@ -578,7 +587,7 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -589,7 +598,7 @@
         <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -627,10 +636,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
@@ -638,48 +647,48 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -691,7 +700,7 @@
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2"/>
     </row>

</xml_diff>